<commit_message>
Adding Sign in tests and Registration form test
</commit_message>
<xml_diff>
--- a/data/AutomationTestPlan.xlsx
+++ b/data/AutomationTestPlan.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="1" r:id="rId1"/>
     <sheet name="TSu1" sheetId="4" r:id="rId2"/>
     <sheet name="TSu2" sheetId="5" r:id="rId3"/>
     <sheet name="TSu3" sheetId="6" r:id="rId4"/>
+    <sheet name="TSu4" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,10 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
-  <si>
-    <t>Precondition:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="118">
   <si>
     <t>Navigate to:</t>
   </si>
@@ -69,27 +67,12 @@
     <t>Sekulic</t>
   </si>
   <si>
-    <t>Insert email into "Email address" input field in the bottom left corner</t>
-  </si>
-  <si>
     <t>Drage Spasic</t>
   </si>
   <si>
     <t>4.</t>
   </si>
   <si>
-    <t>Insert first name into "First name" input field</t>
-  </si>
-  <si>
-    <t>Insert last name into "Last name" input field</t>
-  </si>
-  <si>
-    <t>Insert address into "Address" input field</t>
-  </si>
-  <si>
-    <t>Insert city into "City" input field</t>
-  </si>
-  <si>
     <t>Novi Sad</t>
   </si>
   <si>
@@ -102,21 +85,12 @@
     <t>6.</t>
   </si>
   <si>
-    <t>Insert postal code into "ZIP/Postal code" input field</t>
-  </si>
-  <si>
     <t>Select state from drop down menu</t>
   </si>
   <si>
     <t>7.</t>
   </si>
   <si>
-    <t>Insert mobile phone into "Mobile phone" input field</t>
-  </si>
-  <si>
-    <t>Insert into "Assign an address alias for future reference" input field</t>
-  </si>
-  <si>
     <t>D. Spasic</t>
   </si>
   <si>
@@ -138,15 +112,9 @@
     <t>12.</t>
   </si>
   <si>
-    <t>Insert password into "Password" input field</t>
-  </si>
-  <si>
     <t>kalininamama</t>
   </si>
   <si>
-    <t>Verify that user can create account with valid email and register by filling all the required fields</t>
-  </si>
-  <si>
     <t>Navigation to "My account" page.</t>
   </si>
   <si>
@@ -156,9 +124,6 @@
     <t>An account using this email address has already been registered. Please enter a valid password or request a new one.</t>
   </si>
   <si>
-    <t>Insert email that belongs to registered account into "Email address" input field in the bottom left corner</t>
-  </si>
-  <si>
     <t>Section</t>
   </si>
   <si>
@@ -186,78 +151,45 @@
     <t>Test case name:</t>
   </si>
   <si>
-    <t>ID1</t>
-  </si>
-  <si>
-    <t>ID2</t>
-  </si>
-  <si>
     <t>Sign in</t>
   </si>
   <si>
     <t>Verify that user can't create account with invalid email address</t>
   </si>
   <si>
-    <t>Verify that user can create account with valid email address and register by filling all the required fields</t>
-  </si>
-  <si>
-    <t>ID3</t>
-  </si>
-  <si>
-    <t>Insert invalid email address into "Email address" input field in the bottom left corner</t>
-  </si>
-  <si>
     <t>ninkovic@y</t>
   </si>
   <si>
     <t>Invalid email address.</t>
   </si>
   <si>
-    <t>Alert:</t>
-  </si>
-  <si>
     <t>TSu2</t>
   </si>
   <si>
     <t>Verify that user can sign in with valid credentials</t>
   </si>
   <si>
-    <t>Input valid email address into "Email address" input field in the bottom right coner</t>
-  </si>
-  <si>
     <t>ninkovicdragana@yahoo.com</t>
   </si>
   <si>
-    <t>Input valid password into "Password" field</t>
-  </si>
-  <si>
     <t>Click on "Sign in" button</t>
   </si>
   <si>
     <t>Verify that user can't sign in with invalid email address</t>
   </si>
   <si>
-    <t>Input invalid email address into "Email address" input field in the bottom right coner</t>
-  </si>
-  <si>
     <t>ninkovic@yah</t>
   </si>
   <si>
     <t>Verify that user can't sign in with invalid password</t>
   </si>
   <si>
-    <t>Input invalid password into "Password" field</t>
-  </si>
-  <si>
     <t>kalina</t>
   </si>
   <si>
     <t>Authentication failed.</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>Verify that only one radio button can be checked at the same time</t>
   </si>
   <si>
@@ -277,6 +209,174 @@
   </si>
   <si>
     <t>ninkovicdragana+12@yahoo.com</t>
+  </si>
+  <si>
+    <t>Personal Information form</t>
+  </si>
+  <si>
+    <t>Check value in the "First name" field</t>
+  </si>
+  <si>
+    <t>Check value in the "Last name" field</t>
+  </si>
+  <si>
+    <t>Check value in the "Email" field</t>
+  </si>
+  <si>
+    <t>Confirm new password into "Confirmation" input field</t>
+  </si>
+  <si>
+    <t>Click on the "Save" button</t>
+  </si>
+  <si>
+    <t>Click on the "Sign out" button</t>
+  </si>
+  <si>
+    <t>Verify that user can create account with valid email address and register by filling all the mandatory fields</t>
+  </si>
+  <si>
+    <t>Verify that user can create account with valid email and register by filling all the mandatory fields</t>
+  </si>
+  <si>
+    <t>Pre-condition:</t>
+  </si>
+  <si>
+    <t>Alert message:</t>
+  </si>
+  <si>
+    <t>User isn't sign in. Expected alert message is:</t>
+  </si>
+  <si>
+    <t>Verify that user can change the password and then sign in with the new password</t>
+  </si>
+  <si>
+    <t>Enter email into "Email address" input field in the bottom left corner</t>
+  </si>
+  <si>
+    <t>Enter first name into "First name" input field</t>
+  </si>
+  <si>
+    <t>Enter last name into "Last name" input field</t>
+  </si>
+  <si>
+    <t>Enter password into "Password" input field</t>
+  </si>
+  <si>
+    <t>Enter address into "Address" input field</t>
+  </si>
+  <si>
+    <t>Enter city into "City" input field</t>
+  </si>
+  <si>
+    <t>Enter postal code into "ZIP/Postal code" input field</t>
+  </si>
+  <si>
+    <t>Enter mobile phone into "Mobile phone" input field</t>
+  </si>
+  <si>
+    <t>Enter address alias into "Assign an address alias for future reference" input field</t>
+  </si>
+  <si>
+    <t>Enter email that belongs to registered account into "Email address" input field in the bottom left corner</t>
+  </si>
+  <si>
+    <t>Enter invalid email address into "Email address" input field in the bottom left corner</t>
+  </si>
+  <si>
+    <t>Enter valid email address into "Email address" input field in the bottom right coner</t>
+  </si>
+  <si>
+    <t>Enter valid password into "Password" field</t>
+  </si>
+  <si>
+    <t>Enter invalid email address into "Email address" input field in the bottom right coner</t>
+  </si>
+  <si>
+    <t>Enter invalid password into "Password" field</t>
+  </si>
+  <si>
+    <t>Enter valid password into "Current password" input field</t>
+  </si>
+  <si>
+    <t>Enter new password into "New password" input field</t>
+  </si>
+  <si>
+    <t>Enter new password into "Password" field</t>
+  </si>
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Verify that user can't sign in if "Email" and "Password" input fields are left blank</t>
+  </si>
+  <si>
+    <t>Verify that fields "First name", "Last name" and "Email" are correctly autofilled in "My personal information" section, after Signing in</t>
+  </si>
+  <si>
+    <t>Verify that fields "First name", "Last name" and "Email" are correctly autofilled in "My personal information" section,  after Signing in</t>
+  </si>
+  <si>
+    <t>Leave the "Email" input field blank</t>
+  </si>
+  <si>
+    <t>Leave the "Password" input field blank</t>
+  </si>
+  <si>
+    <t>An email address required.</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>Verify that there is no result if "Search" box is blank and "Search" button is clicked</t>
+  </si>
+  <si>
+    <t>TSu4</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>Leave "Search" field blank</t>
+  </si>
+  <si>
+    <t>Click on "Search" button</t>
+  </si>
+  <si>
+    <t>0 results have been found.</t>
+  </si>
+  <si>
+    <t>There isn't any found product. Notification is displayed, with text:</t>
   </si>
 </sst>
 </file>
@@ -365,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -414,16 +514,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -706,158 +818,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="84.6640625" customWidth="1"/>
+    <col min="2" max="2" width="88" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="24"/>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="D6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="B12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -868,152 +1069,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.21875" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="D17" s="3">
         <v>21000</v>
@@ -1021,10 +1222,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5">
         <v>381642636375</v>
@@ -1032,72 +1233,72 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
         <v>0</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D31" t="str">
         <f>D9</f>
@@ -1106,10 +1307,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
         <v>8</v>
-      </c>
-      <c r="C32" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1117,67 +1318,67 @@
     </row>
     <row r="34" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
         <v>0</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
         <v>8</v>
-      </c>
-      <c r="C44" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1185,13 +1386,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1205,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1221,353 +1422,831 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>65</v>
+        <v>97</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
         <v>0</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="D20" t="s">
         <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>88</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>10</v>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="13"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
+      <c r="D26" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" s="17"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s">
-        <v>76</v>
+      <c r="C49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
-    <hyperlink ref="D20" r:id="rId2"/>
-    <hyperlink ref="D32" r:id="rId3"/>
+    <hyperlink ref="D22" r:id="rId1"/>
+    <hyperlink ref="D35" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B7" sqref="B7:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
     <col min="3" max="3" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="str">
+        <f>'TSu1'!D11</f>
+        <v>Dragana</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" t="str">
+        <f>'TSu1'!D12</f>
+        <v>Sekulic</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="str">
+        <f>'TSu3'!D26</f>
+        <v>ninkovicdragana@yahoo.com</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" t="str">
+        <f>D41</f>
+        <v>kalininamama</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D26" r:id="rId2"/>
+    <hyperlink ref="D40" r:id="rId3"/>
+    <hyperlink ref="D49" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>78</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>17</v>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
+        <v>117</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>